<commit_message>
24v wire harness directions
</commit_message>
<xml_diff>
--- a/Antonio-Feed/Wiring Harnesses/Feed/24v to Control Board Cable/List of materials (24v).xlsx
+++ b/Antonio-Feed/Wiring Harnesses/Feed/24v to Control Board Cable/List of materials (24v).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarahschoultz/Documents/GitHub/Front-Page/Antonio-Feed/Wiring Harnesses/Feed/24v to Control Board Cable/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarah/Documents/Wiring Harness Directions/24v to Control Board Cable/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BFC9478-4778-2A49-B396-BC3B2AA058DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9439DB61-94DF-244F-A577-F97995A927FD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2620" yWindow="460" windowWidth="20020" windowHeight="13860" xr2:uid="{1354B1EE-61B1-EA40-838A-2C3EED4877E0}"/>
+    <workbookView xWindow="9280" yWindow="2500" windowWidth="23880" windowHeight="15680" xr2:uid="{1354B1EE-61B1-EA40-838A-2C3EED4877E0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="86">
   <si>
     <t>Material</t>
   </si>
@@ -66,12 +66,6 @@
     <t>Order Number of Distributor</t>
   </si>
   <si>
-    <t>Shrink tube</t>
-  </si>
-  <si>
-    <t>Metal braid</t>
-  </si>
-  <si>
     <t>Plastic braid</t>
   </si>
   <si>
@@ -87,12 +81,6 @@
     <t>Red 14 awg</t>
   </si>
   <si>
-    <t>Eyeconnector</t>
-  </si>
-  <si>
-    <t>Fork 16-14 AWG</t>
-  </si>
-  <si>
     <t>Wire tips</t>
   </si>
   <si>
@@ -168,18 +156,6 @@
     <t>Stripping wires to attach tips</t>
   </si>
   <si>
-    <t>Fork crimper</t>
-  </si>
-  <si>
-    <t>Crimping on fork tips</t>
-  </si>
-  <si>
-    <t>Eye crimper</t>
-  </si>
-  <si>
-    <t>Crimping on eye tips</t>
-  </si>
-  <si>
     <t>ALPHA WIRE</t>
   </si>
   <si>
@@ -231,9 +207,6 @@
     <t>Tip soder joint covers</t>
   </si>
   <si>
-    <t>1 in</t>
-  </si>
-  <si>
     <t>TE Connectivity / Raychem</t>
   </si>
   <si>
@@ -244,13 +217,88 @@
   </si>
   <si>
     <t>09J3954</t>
+  </si>
+  <si>
+    <t>6.4mm in adehsive shrink tube</t>
+  </si>
+  <si>
+    <t>TAT-125-1/4-0-STK</t>
+  </si>
+  <si>
+    <t>650-TAT125014</t>
+  </si>
+  <si>
+    <t>Metal Braid</t>
+  </si>
+  <si>
+    <t>42in</t>
+  </si>
+  <si>
+    <t>17in</t>
+  </si>
+  <si>
+    <t>.203 Metal Braid</t>
+  </si>
+  <si>
+    <t>Glenari</t>
+  </si>
+  <si>
+    <t>100-001A203</t>
+  </si>
+  <si>
+    <t>654-100001A203</t>
+  </si>
+  <si>
+    <t>27.5in</t>
+  </si>
+  <si>
+    <t>1.5in</t>
+  </si>
+  <si>
+    <t>12.7mm adhesive shrink tube</t>
+  </si>
+  <si>
+    <t>1.75in</t>
+  </si>
+  <si>
+    <t>DWP-125-1/2-0-STK</t>
+  </si>
+  <si>
+    <t>650-DWP-125-1/2-0</t>
+  </si>
+  <si>
+    <t>28in</t>
+  </si>
+  <si>
+    <t>2 in</t>
+  </si>
+  <si>
+    <t>8 Eye connector</t>
+  </si>
+  <si>
+    <t>6 Fork connector</t>
+  </si>
+  <si>
+    <t>Fork &amp; Eye crimper</t>
+  </si>
+  <si>
+    <t>Crimping on fork &amp; eye tips</t>
+  </si>
+  <si>
+    <t>517-2224</t>
+  </si>
+  <si>
+    <t>(11-8)</t>
+  </si>
+  <si>
+    <t>3M Electronic Specialty</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -281,20 +329,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FFFFC000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF333333"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -316,15 +350,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -647,7 +680,7 @@
   <dimension ref="A1:M15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:G11"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -663,16 +696,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
@@ -684,258 +717,325 @@
       <c r="G1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="L2" t="s">
+        <v>21</v>
+      </c>
+      <c r="M2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="6"/>
+      <c r="C3" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="L3" t="s">
+        <v>53</v>
+      </c>
+      <c r="M3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="L4" t="s">
+        <v>23</v>
+      </c>
+      <c r="M4" t="s">
         <v>24</v>
       </c>
-      <c r="M1" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="L5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="L6" t="s">
+        <v>27</v>
+      </c>
+      <c r="M6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="L7" t="s">
+        <v>49</v>
+      </c>
+      <c r="M7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="L8" t="s">
+        <v>29</v>
+      </c>
+      <c r="M8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="4">
+        <v>2</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="L2" t="s">
-        <v>25</v>
-      </c>
-      <c r="M2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="s">
+      <c r="E9" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="L9" t="s">
+        <v>31</v>
+      </c>
+      <c r="M9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="7"/>
-      <c r="D3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="L3" t="s">
-        <v>61</v>
-      </c>
-      <c r="M3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" t="s">
-        <v>48</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="L4" t="s">
-        <v>27</v>
-      </c>
-      <c r="M4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" t="s">
-        <v>14</v>
-      </c>
-      <c r="L5" t="s">
-        <v>29</v>
-      </c>
-      <c r="M5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="C10" s="4">
+        <v>2</v>
+      </c>
+      <c r="D10" t="s">
+        <v>85</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="L10" t="s">
+        <v>33</v>
+      </c>
+      <c r="M10" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="B11" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="E6" t="s">
+      <c r="C11" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F11" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G11" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="G6" t="s">
-        <v>59</v>
-      </c>
-      <c r="L6" t="s">
-        <v>31</v>
-      </c>
-      <c r="M6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" t="s">
-        <v>11</v>
-      </c>
-      <c r="L7" t="s">
-        <v>57</v>
-      </c>
-      <c r="M7" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" t="s">
-        <v>12</v>
-      </c>
-      <c r="L8" t="s">
-        <v>33</v>
-      </c>
-      <c r="M8" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9">
-        <v>2</v>
-      </c>
-      <c r="D9" t="s">
-        <v>20</v>
-      </c>
-      <c r="E9" t="s">
-        <v>21</v>
-      </c>
-      <c r="F9" t="s">
-        <v>22</v>
-      </c>
-      <c r="G9" t="s">
-        <v>23</v>
-      </c>
-      <c r="L9" t="s">
+      <c r="L11" t="s">
         <v>35</v>
       </c>
-      <c r="M9" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10">
-        <v>2</v>
-      </c>
-      <c r="L10" t="s">
-        <v>37</v>
-      </c>
-      <c r="M10" s="8" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>63</v>
-      </c>
-      <c r="B11" t="s">
-        <v>64</v>
-      </c>
-      <c r="C11" t="s">
-        <v>65</v>
-      </c>
-      <c r="D11" t="s">
-        <v>66</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="F11" t="s">
-        <v>68</v>
-      </c>
-      <c r="G11" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="L11" t="s">
-        <v>39</v>
-      </c>
-      <c r="M11" s="8"/>
+      <c r="M11" s="7"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="L12" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="M12" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="L13" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="M13" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="L14" s="5" t="s">
-        <v>44</v>
+      <c r="L14" s="4" t="s">
+        <v>81</v>
       </c>
       <c r="M14" t="s">
-        <v>45</v>
+        <v>82</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="L15" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="M15" t="s">
-        <v>47</v>
-      </c>
+      <c r="L15" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>